<commit_message>
Changes for ledger types validations
Changes for ledger types validations
</commit_message>
<xml_diff>
--- a/01_Requirements/Lists_Individual.xlsx
+++ b/01_Requirements/Lists_Individual.xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\narendar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\IIT\01_Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Group_subGroup" sheetId="1" r:id="rId1"/>
+    <sheet name="Ledgertypes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="96">
   <si>
     <t>Head</t>
   </si>
@@ -51,9 +52,6 @@
     <t>Fixed Assets</t>
   </si>
   <si>
-    <t>Lands</t>
-  </si>
-  <si>
     <t>Buildings</t>
   </si>
   <si>
@@ -295,6 +293,33 @@
   </si>
   <si>
     <t>Indirect Income</t>
+  </si>
+  <si>
+    <t>LedgerType</t>
+  </si>
+  <si>
+    <t>Bank Account</t>
+  </si>
+  <si>
+    <t>Capital Account</t>
+  </si>
+  <si>
+    <t>CC / ODC</t>
+  </si>
+  <si>
+    <t>Creditors</t>
+  </si>
+  <si>
+    <t>Debtors</t>
+  </si>
+  <si>
+    <t>Investment</t>
+  </si>
+  <si>
+    <t>Services or Dues to Sub-contractors</t>
+  </si>
+  <si>
+    <t>Default</t>
   </si>
 </sst>
 </file>
@@ -723,7 +748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -752,7 +777,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75">
@@ -763,7 +788,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2">
@@ -778,7 +803,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3">
@@ -793,7 +818,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4">
@@ -808,7 +833,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5">
@@ -823,7 +848,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6">
@@ -838,7 +863,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7">
@@ -853,7 +878,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8">
@@ -868,7 +893,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9">
@@ -883,7 +908,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10">
@@ -898,7 +923,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11">
@@ -913,7 +938,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12">
@@ -925,10 +950,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13">
@@ -940,10 +965,10 @@
         <v>4</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14">
@@ -955,10 +980,10 @@
         <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15">
@@ -970,10 +995,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16">
@@ -985,10 +1010,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17">
@@ -1000,10 +1025,10 @@
         <v>4</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18">
@@ -1015,10 +1040,10 @@
         <v>4</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19">
@@ -1030,10 +1055,10 @@
         <v>4</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20">
@@ -1045,10 +1070,10 @@
         <v>4</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21">
@@ -1060,10 +1085,10 @@
         <v>4</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22">
@@ -1075,10 +1100,10 @@
         <v>4</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23">
@@ -1090,13 +1115,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E24">
         <v>24</v>
@@ -1107,10 +1132,10 @@
         <v>4</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25">
@@ -1122,10 +1147,10 @@
         <v>4</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26">
@@ -1137,10 +1162,10 @@
         <v>4</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27">
@@ -1152,10 +1177,10 @@
         <v>4</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28">
@@ -1167,10 +1192,10 @@
         <v>4</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29">
@@ -1182,10 +1207,10 @@
         <v>4</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30">
@@ -1197,10 +1222,10 @@
         <v>4</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31">
@@ -1212,10 +1237,10 @@
         <v>4</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32">
@@ -1227,10 +1252,10 @@
         <v>4</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33">
@@ -1242,10 +1267,10 @@
         <v>4</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34">
@@ -1257,10 +1282,10 @@
         <v>4</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35">
@@ -1272,10 +1297,10 @@
         <v>4</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36">
@@ -1287,10 +1312,10 @@
         <v>4</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37">
@@ -1299,16 +1324,16 @@
     </row>
     <row r="38" spans="1:5" ht="15.75">
       <c r="A38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="E38">
         <v>38</v>
@@ -1316,13 +1341,13 @@
     </row>
     <row r="39" spans="1:5" ht="15.75">
       <c r="A39" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39">
@@ -1331,13 +1356,13 @@
     </row>
     <row r="40" spans="1:5" ht="15.75">
       <c r="A40" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40">
@@ -1346,13 +1371,13 @@
     </row>
     <row r="41" spans="1:5" ht="15.75">
       <c r="A41" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41">
@@ -1361,13 +1386,13 @@
     </row>
     <row r="42" spans="1:5" ht="15.75">
       <c r="A42" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42">
@@ -1376,13 +1401,13 @@
     </row>
     <row r="43" spans="1:5" ht="15.75">
       <c r="A43" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43">
@@ -1391,13 +1416,13 @@
     </row>
     <row r="44" spans="1:5" ht="15.75">
       <c r="A44" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44">
@@ -1406,13 +1431,13 @@
     </row>
     <row r="45" spans="1:5" ht="15.75">
       <c r="A45" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45">
@@ -1421,13 +1446,13 @@
     </row>
     <row r="46" spans="1:5" ht="15.75">
       <c r="A46" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46">
@@ -1436,13 +1461,13 @@
     </row>
     <row r="47" spans="1:5" ht="15.75">
       <c r="A47" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47">
@@ -1451,13 +1476,13 @@
     </row>
     <row r="48" spans="1:5" ht="15.75">
       <c r="A48" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48">
@@ -1466,13 +1491,13 @@
     </row>
     <row r="49" spans="1:5" ht="15.75">
       <c r="A49" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49">
@@ -1481,13 +1506,13 @@
     </row>
     <row r="50" spans="1:5" ht="15.75">
       <c r="A50" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50">
@@ -1496,13 +1521,13 @@
     </row>
     <row r="51" spans="1:5" ht="15.75">
       <c r="A51" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51">
@@ -1511,13 +1536,13 @@
     </row>
     <row r="52" spans="1:5" ht="15.75">
       <c r="A52" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52">
@@ -1526,13 +1551,13 @@
     </row>
     <row r="53" spans="1:5" ht="15.75">
       <c r="A53" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53">
@@ -1541,16 +1566,16 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="C54" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="D54" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="E54">
         <v>54</v>
@@ -1558,16 +1583,16 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="C55" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="D55" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E55">
         <v>55</v>
@@ -1575,16 +1600,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="C56" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="D56" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E56">
         <v>56</v>
@@ -1592,16 +1617,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B57" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="E57">
         <v>57</v>
@@ -1609,13 +1634,13 @@
     </row>
     <row r="58" spans="1:5" ht="15.75">
       <c r="A58" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="C58" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58">
@@ -1624,13 +1649,13 @@
     </row>
     <row r="59" spans="1:5" ht="15.75">
       <c r="A59" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="C59" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59">
@@ -1639,13 +1664,13 @@
     </row>
     <row r="60" spans="1:5" ht="15.75">
       <c r="A60" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="C60" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60">
@@ -1654,13 +1679,13 @@
     </row>
     <row r="61" spans="1:5" ht="15.75">
       <c r="A61" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B61" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61">
@@ -1669,13 +1694,13 @@
     </row>
     <row r="62" spans="1:5" ht="15.75">
       <c r="A62" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62">
@@ -1684,17 +1709,147 @@
     </row>
     <row r="63" spans="1:5" ht="15.75">
       <c r="A63" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63">
         <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>68</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>70</v>
+      </c>
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>